<commit_message>
Aggiustato printing/output + Aggiustato come funzionava check_LS
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/sequenza_post.xlsx
+++ b/PS-VRP/Dati_output/sequenza_post.xlsx
@@ -434,11 +434,13 @@
     <col width="50" customWidth="1" min="8" max="8"/>
     <col width="15" customWidth="1" min="9" max="9"/>
     <col width="15" customWidth="1" min="10" max="10"/>
-    <col width="100" customWidth="1" min="11" max="11"/>
+    <col width="90" customWidth="1" min="11" max="11"/>
     <col width="15" customWidth="1" min="12" max="12"/>
     <col width="15" customWidth="1" min="13" max="13"/>
     <col width="15" customWidth="1" min="14" max="14"/>
     <col width="15" customWidth="1" min="15" max="15"/>
+    <col width="15" customWidth="1" min="16" max="16"/>
+    <col width="20" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -512,6 +514,31 @@
           <t>veicolo</t>
         </is>
       </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>tassativita</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>veicolo tassativo</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>due date (non indicativa)</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>ritardo</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>priorita</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">

</xml_diff>